<commit_message>
Comments, Registration Redesign (WIP), and Etc
</commit_message>
<xml_diff>
--- a/Timesheets/kjohnson/kjohnson11.xlsx
+++ b/Timesheets/kjohnson/kjohnson11.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Senior Project - Spring / Summer 2015</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Time sheets, team communication</t>
+  </si>
+  <si>
+    <t>3:00pm – 4:45</t>
+  </si>
+  <si>
+    <t>Registration page reconstruction, code documentation, questions stuff</t>
   </si>
 </sst>
 </file>
@@ -230,7 +236,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -315,9 +321,15 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>

</xml_diff>